<commit_message>
Update CDC cases projection 2022-02-19.xlsx
</commit_message>
<xml_diff>
--- a/data/CDC cases projection 2022-02-19.xlsx
+++ b/data/CDC cases projection 2022-02-19.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matt_\GitHub\covid-wisconsin\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{EC069EAF-EA59-4B38-A519-FDE389686D93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{2D25E4E8-0C31-4FE9-B219-AAFBAD037B89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
@@ -5995,8 +5995,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G770"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D19" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>